<commit_message>
merge all working test cases over
</commit_message>
<xml_diff>
--- a/data/NGQ_US9400_04_data.xlsx
+++ b/data/NGQ_US9400_04_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huntejos\NGQ\ngq-test-scripts\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huntejos\NGQ\NGQ\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Opportunity_ID</t>
   </si>
@@ -36,16 +36,98 @@
   </si>
   <si>
     <t>OPE-0002907630</t>
+  </si>
+  <si>
+    <t>uploadConfigPath</t>
+  </si>
+  <si>
+    <t>727021-B21</t>
+  </si>
+  <si>
+    <t>HP BL460c Gen9 10Gb/20Gb FLB CTO Blade</t>
+  </si>
+  <si>
+    <t>726991-L21</t>
+  </si>
+  <si>
+    <t>HP BL460c Gen9 E5-2650v3 FIO Kit</t>
+  </si>
+  <si>
+    <t>726991-B21</t>
+  </si>
+  <si>
+    <t>HP BL460c Gen9 E5-2650v3 Kit</t>
+  </si>
+  <si>
+    <t>726722-B21</t>
+  </si>
+  <si>
+    <t>HP 32GB 4Rx4 PC4-2133P-L Kit</t>
+  </si>
+  <si>
+    <t>700764-B21</t>
+  </si>
+  <si>
+    <t>H1K92A3</t>
+  </si>
+  <si>
+    <t>HA114A1</t>
+  </si>
+  <si>
+    <t>productNum</t>
+  </si>
+  <si>
+    <t>productDesc</t>
+  </si>
+  <si>
+    <t>productOpt</t>
+  </si>
+  <si>
+    <t>0D1</t>
+  </si>
+  <si>
+    <t>TT8</t>
+  </si>
+  <si>
+    <t>5CY</t>
+  </si>
+  <si>
+    <t>HP CP Installation &amp; Startup</t>
+  </si>
+  <si>
+    <t>HPE 3Y Proactive Care 24x7 SVC</t>
+  </si>
+  <si>
+    <t>HP C Class Server Blade Startup SVC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>DESSTEPS_335038_CPQ Encore_US9400_04_config.xls</t>
+  </si>
+  <si>
+    <t>HP FlexFabric 20Gb 2P 650FLB FIO Adptr</t>
+  </si>
+  <si>
+    <t>HP BL460c Gen9 Server Blade HW Supp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -71,8 +153,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -353,35 +437,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="84" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>